<commit_message>
v2p14. Compatible with MF-Swift v2212, updated hardpoints.
</commit_message>
<xml_diff>
--- a/Libraries/Vehicle/AntiRollBar/sm_car_data_AntiRollBar_Droplink.xlsx
+++ b/Libraries/Vehicle/AntiRollBar/sm_car_data_AntiRollBar_Droplink.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT\Others\smiller\ssvt\Libraries\Vehicle\AntiRollBar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D045DC36-EDE4-4096-88BA-3751E43B2F41}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6140A5AC-C4E1-46F9-A3F6-E98E6744DC41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="9072" tabRatio="979" xr2:uid="{3FA59F9D-D9D3-4E28-B3CE-9BFC80E89258}"/>
+    <workbookView xWindow="29850" yWindow="1050" windowWidth="21600" windowHeight="12915" tabRatio="979" activeTab="6" xr2:uid="{3FA59F9D-D9D3-4E28-B3CE-9BFC80E89258}"/>
   </bookViews>
   <sheets>
     <sheet name="Sedan_HambaLG_f" sheetId="12" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="Sedan_Hamba_r" sheetId="13" r:id="rId4"/>
     <sheet name="Bus_Makulu_f" sheetId="9" r:id="rId5"/>
     <sheet name="Bus_Makulu_r" sheetId="10" r:id="rId6"/>
+    <sheet name="Trailer1Axle_f" sheetId="15" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -28,7 +29,12 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -36,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="23">
   <si>
     <t>Units</t>
   </si>
@@ -102,6 +108,9 @@
   </si>
   <si>
     <t>Droplink_Bus_Makhulu_r</t>
+  </si>
+  <si>
+    <t>Droplink_Trailer1Axle_f</t>
   </si>
 </sst>
 </file>
@@ -202,7 +211,35 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="24">
+  <dxfs count="28">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -673,7 +710,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -686,7 +723,7 @@
   </sheetPr>
   <dimension ref="A1:AB15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="D33" sqref="D33"/>
       <selection pane="topRight" activeCell="D33" sqref="D33"/>
@@ -694,17 +731,17 @@
       <selection pane="bottomRight" activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" style="14" customWidth="1"/>
-    <col min="2" max="2" width="12.77734375" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" customWidth="1"/>
-    <col min="4" max="4" width="11.109375" customWidth="1"/>
-    <col min="5" max="5" width="16.6640625" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" style="14" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" customWidth="1"/>
     <col min="6" max="8" width="10" customWidth="1"/>
-    <col min="9" max="15" width="6.6640625" customWidth="1"/>
-    <col min="16" max="16" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="15" width="6.7109375" customWidth="1"/>
+    <col min="16" max="16" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="6.7109375" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="2" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="6" bestFit="1" customWidth="1"/>
     <col min="20" max="26" width="7" bestFit="1" customWidth="1"/>
@@ -712,7 +749,7 @@
     <col min="28" max="28" width="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
       <c r="C1" s="3"/>
@@ -732,7 +769,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
@@ -746,7 +783,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
@@ -760,7 +797,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>7</v>
       </c>
@@ -793,7 +830,7 @@
       <c r="AA4"/>
       <c r="AB4"/>
     </row>
-    <row r="5" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>11</v>
       </c>
@@ -810,7 +847,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="6" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>13</v>
       </c>
@@ -827,7 +864,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="7" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>9</v>
       </c>
@@ -840,7 +877,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>12</v>
       </c>
@@ -853,66 +890,66 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="9" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="12"/>
       <c r="F9" s="7"/>
       <c r="G9" s="7"/>
       <c r="H9" s="7"/>
     </row>
-    <row r="10" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="12"/>
       <c r="B10" s="12"/>
       <c r="F10" s="7"/>
       <c r="G10" s="7"/>
       <c r="H10" s="7"/>
     </row>
-    <row r="11" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="12"/>
       <c r="B11" s="12"/>
       <c r="F11" s="7"/>
       <c r="G11" s="7"/>
       <c r="H11" s="7"/>
     </row>
-    <row r="12" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="12"/>
       <c r="F12" s="7"/>
       <c r="G12" s="7"/>
       <c r="H12" s="7"/>
     </row>
-    <row r="13" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12"/>
       <c r="F13" s="7"/>
       <c r="G13" s="7"/>
       <c r="H13" s="7"/>
     </row>
-    <row r="14" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="12"/>
       <c r="B14" s="12"/>
       <c r="H14" s="13"/>
     </row>
-    <row r="15" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="12"/>
       <c r="B15" s="12"/>
       <c r="H15" s="13"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A12:B13">
-    <cfRule type="cellIs" dxfId="23" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="4" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A14">
-    <cfRule type="cellIs" dxfId="22" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="2" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A10:B11 A4:B4">
-    <cfRule type="cellIs" dxfId="21" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="3" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A15">
-    <cfRule type="cellIs" dxfId="20" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="1" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -935,17 +972,17 @@
       <selection pane="bottomRight" activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" style="14" customWidth="1"/>
-    <col min="2" max="2" width="12.77734375" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" customWidth="1"/>
-    <col min="4" max="4" width="11.109375" customWidth="1"/>
-    <col min="5" max="5" width="16.6640625" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" style="14" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" customWidth="1"/>
     <col min="6" max="8" width="10" customWidth="1"/>
-    <col min="9" max="15" width="6.6640625" customWidth="1"/>
-    <col min="16" max="16" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="15" width="6.7109375" customWidth="1"/>
+    <col min="16" max="16" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="6.7109375" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="2" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="6" bestFit="1" customWidth="1"/>
     <col min="20" max="26" width="7" bestFit="1" customWidth="1"/>
@@ -953,7 +990,7 @@
     <col min="28" max="28" width="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
       <c r="C1" s="3"/>
@@ -973,7 +1010,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
@@ -987,7 +1024,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
@@ -1001,7 +1038,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>7</v>
       </c>
@@ -1034,7 +1071,7 @@
       <c r="AA4"/>
       <c r="AB4"/>
     </row>
-    <row r="5" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>11</v>
       </c>
@@ -1051,7 +1088,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="6" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>13</v>
       </c>
@@ -1068,7 +1105,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="7" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>9</v>
       </c>
@@ -1081,7 +1118,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>12</v>
       </c>
@@ -1094,66 +1131,66 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="9" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="12"/>
       <c r="F9" s="7"/>
       <c r="G9" s="7"/>
       <c r="H9" s="7"/>
     </row>
-    <row r="10" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="12"/>
       <c r="B10" s="12"/>
       <c r="F10" s="7"/>
       <c r="G10" s="7"/>
       <c r="H10" s="7"/>
     </row>
-    <row r="11" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="12"/>
       <c r="B11" s="12"/>
       <c r="F11" s="7"/>
       <c r="G11" s="7"/>
       <c r="H11" s="7"/>
     </row>
-    <row r="12" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="12"/>
       <c r="F12" s="7"/>
       <c r="G12" s="7"/>
       <c r="H12" s="7"/>
     </row>
-    <row r="13" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12"/>
       <c r="F13" s="7"/>
       <c r="G13" s="7"/>
       <c r="H13" s="7"/>
     </row>
-    <row r="14" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="12"/>
       <c r="B14" s="12"/>
       <c r="H14" s="13"/>
     </row>
-    <row r="15" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="12"/>
       <c r="B15" s="12"/>
       <c r="H15" s="13"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A12:B13">
-    <cfRule type="cellIs" dxfId="19" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="4" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A14">
-    <cfRule type="cellIs" dxfId="18" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="2" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A10:B11 A4:B4">
-    <cfRule type="cellIs" dxfId="17" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="3" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A15">
-    <cfRule type="cellIs" dxfId="16" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="1" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1176,17 +1213,17 @@
       <selection pane="bottomRight" activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" style="14" customWidth="1"/>
-    <col min="2" max="2" width="12.77734375" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" customWidth="1"/>
-    <col min="4" max="4" width="11.109375" customWidth="1"/>
-    <col min="5" max="5" width="16.6640625" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" style="14" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" customWidth="1"/>
     <col min="6" max="8" width="10" customWidth="1"/>
-    <col min="9" max="15" width="6.6640625" customWidth="1"/>
-    <col min="16" max="16" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="15" width="6.7109375" customWidth="1"/>
+    <col min="16" max="16" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="6.7109375" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="2" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="6" bestFit="1" customWidth="1"/>
     <col min="20" max="26" width="7" bestFit="1" customWidth="1"/>
@@ -1194,7 +1231,7 @@
     <col min="28" max="28" width="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
       <c r="C1" s="3"/>
@@ -1214,7 +1251,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
@@ -1228,7 +1265,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
@@ -1242,7 +1279,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>7</v>
       </c>
@@ -1275,7 +1312,7 @@
       <c r="AA4"/>
       <c r="AB4"/>
     </row>
-    <row r="5" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>11</v>
       </c>
@@ -1292,7 +1329,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="6" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>13</v>
       </c>
@@ -1309,7 +1346,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="7" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>9</v>
       </c>
@@ -1322,7 +1359,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>12</v>
       </c>
@@ -1335,66 +1372,66 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="9" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="12"/>
       <c r="F9" s="7"/>
       <c r="G9" s="7"/>
       <c r="H9" s="7"/>
     </row>
-    <row r="10" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="12"/>
       <c r="B10" s="12"/>
       <c r="F10" s="7"/>
       <c r="G10" s="7"/>
       <c r="H10" s="7"/>
     </row>
-    <row r="11" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="12"/>
       <c r="B11" s="12"/>
       <c r="F11" s="7"/>
       <c r="G11" s="7"/>
       <c r="H11" s="7"/>
     </row>
-    <row r="12" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="12"/>
       <c r="F12" s="7"/>
       <c r="G12" s="7"/>
       <c r="H12" s="7"/>
     </row>
-    <row r="13" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12"/>
       <c r="F13" s="7"/>
       <c r="G13" s="7"/>
       <c r="H13" s="7"/>
     </row>
-    <row r="14" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="12"/>
       <c r="B14" s="12"/>
       <c r="H14" s="13"/>
     </row>
-    <row r="15" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="12"/>
       <c r="B15" s="12"/>
       <c r="H15" s="13"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A12:B13">
-    <cfRule type="cellIs" dxfId="15" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="4" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A14">
-    <cfRule type="cellIs" dxfId="14" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="2" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A10:B11 A4:B4">
-    <cfRule type="cellIs" dxfId="13" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="3" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A15">
-    <cfRule type="cellIs" dxfId="12" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="1" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1417,17 +1454,17 @@
       <selection pane="bottomRight" activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" style="14" customWidth="1"/>
-    <col min="2" max="2" width="12.77734375" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" customWidth="1"/>
-    <col min="4" max="4" width="11.109375" customWidth="1"/>
-    <col min="5" max="5" width="16.6640625" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" style="14" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" customWidth="1"/>
     <col min="6" max="8" width="10" customWidth="1"/>
-    <col min="9" max="15" width="6.6640625" customWidth="1"/>
-    <col min="16" max="16" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="15" width="6.7109375" customWidth="1"/>
+    <col min="16" max="16" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="6.7109375" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="2" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="6" bestFit="1" customWidth="1"/>
     <col min="20" max="26" width="7" bestFit="1" customWidth="1"/>
@@ -1435,7 +1472,7 @@
     <col min="28" max="28" width="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
       <c r="C1" s="3"/>
@@ -1455,7 +1492,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
@@ -1469,7 +1506,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
@@ -1483,7 +1520,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>7</v>
       </c>
@@ -1516,7 +1553,7 @@
       <c r="AA4"/>
       <c r="AB4"/>
     </row>
-    <row r="5" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>11</v>
       </c>
@@ -1533,7 +1570,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="6" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>13</v>
       </c>
@@ -1550,7 +1587,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="7" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>9</v>
       </c>
@@ -1563,7 +1600,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>12</v>
       </c>
@@ -1576,66 +1613,66 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="9" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="12"/>
       <c r="F9" s="7"/>
       <c r="G9" s="7"/>
       <c r="H9" s="7"/>
     </row>
-    <row r="10" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="12"/>
       <c r="B10" s="12"/>
       <c r="F10" s="7"/>
       <c r="G10" s="7"/>
       <c r="H10" s="7"/>
     </row>
-    <row r="11" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="12"/>
       <c r="B11" s="12"/>
       <c r="F11" s="7"/>
       <c r="G11" s="7"/>
       <c r="H11" s="7"/>
     </row>
-    <row r="12" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="12"/>
       <c r="F12" s="7"/>
       <c r="G12" s="7"/>
       <c r="H12" s="7"/>
     </row>
-    <row r="13" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12"/>
       <c r="F13" s="7"/>
       <c r="G13" s="7"/>
       <c r="H13" s="7"/>
     </row>
-    <row r="14" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="12"/>
       <c r="B14" s="12"/>
       <c r="H14" s="13"/>
     </row>
-    <row r="15" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="12"/>
       <c r="B15" s="12"/>
       <c r="H15" s="13"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A12:B13">
-    <cfRule type="cellIs" dxfId="11" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="4" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A14">
-    <cfRule type="cellIs" dxfId="10" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="2" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A10:B11 A4:B4">
-    <cfRule type="cellIs" dxfId="9" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="3" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A15">
-    <cfRule type="cellIs" dxfId="8" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="1" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1658,17 +1695,17 @@
       <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" style="14" customWidth="1"/>
-    <col min="2" max="2" width="12.77734375" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" customWidth="1"/>
-    <col min="4" max="4" width="11.109375" customWidth="1"/>
-    <col min="5" max="5" width="16.6640625" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" style="14" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" customWidth="1"/>
     <col min="6" max="8" width="10" customWidth="1"/>
-    <col min="9" max="15" width="6.6640625" customWidth="1"/>
-    <col min="16" max="16" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="15" width="6.7109375" customWidth="1"/>
+    <col min="16" max="16" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="6.7109375" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="2" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="6" bestFit="1" customWidth="1"/>
     <col min="20" max="26" width="7" bestFit="1" customWidth="1"/>
@@ -1676,7 +1713,7 @@
     <col min="28" max="28" width="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
       <c r="C1" s="3"/>
@@ -1696,7 +1733,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
@@ -1710,7 +1747,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
@@ -1724,7 +1761,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>7</v>
       </c>
@@ -1757,7 +1794,7 @@
       <c r="AA4"/>
       <c r="AB4"/>
     </row>
-    <row r="5" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>11</v>
       </c>
@@ -1774,7 +1811,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="6" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>13</v>
       </c>
@@ -1791,7 +1828,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="7" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>9</v>
       </c>
@@ -1804,7 +1841,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>12</v>
       </c>
@@ -1817,66 +1854,66 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="9" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="12"/>
       <c r="F9" s="7"/>
       <c r="G9" s="7"/>
       <c r="H9" s="7"/>
     </row>
-    <row r="10" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="12"/>
       <c r="B10" s="12"/>
       <c r="F10" s="7"/>
       <c r="G10" s="7"/>
       <c r="H10" s="7"/>
     </row>
-    <row r="11" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="12"/>
       <c r="B11" s="12"/>
       <c r="F11" s="7"/>
       <c r="G11" s="7"/>
       <c r="H11" s="7"/>
     </row>
-    <row r="12" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="12"/>
       <c r="F12" s="7"/>
       <c r="G12" s="7"/>
       <c r="H12" s="7"/>
     </row>
-    <row r="13" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12"/>
       <c r="F13" s="7"/>
       <c r="G13" s="7"/>
       <c r="H13" s="7"/>
     </row>
-    <row r="14" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="12"/>
       <c r="B14" s="12"/>
       <c r="H14" s="13"/>
     </row>
-    <row r="15" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="12"/>
       <c r="B15" s="12"/>
       <c r="H15" s="13"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A12:B13">
-    <cfRule type="cellIs" dxfId="7" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="4" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A14">
-    <cfRule type="cellIs" dxfId="6" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="2" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A10:B11 A4:B4">
-    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="3" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A15">
-    <cfRule type="cellIs" dxfId="4" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="1" operator="equal">
       <formula>"class"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1899,17 +1936,17 @@
       <selection pane="bottomRight" activeCell="V27" sqref="V27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" style="14" customWidth="1"/>
-    <col min="2" max="2" width="12.77734375" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" customWidth="1"/>
-    <col min="4" max="4" width="11.109375" customWidth="1"/>
-    <col min="5" max="5" width="16.6640625" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" style="14" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" customWidth="1"/>
     <col min="6" max="8" width="10" customWidth="1"/>
-    <col min="9" max="15" width="6.6640625" customWidth="1"/>
-    <col min="16" max="16" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="15" width="6.7109375" customWidth="1"/>
+    <col min="16" max="16" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="6.7109375" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="2" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="6" bestFit="1" customWidth="1"/>
     <col min="20" max="26" width="7" bestFit="1" customWidth="1"/>
@@ -1917,7 +1954,7 @@
     <col min="28" max="28" width="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
       <c r="C1" s="3"/>
@@ -1937,7 +1974,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
@@ -1951,7 +1988,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
@@ -1965,7 +2002,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>7</v>
       </c>
@@ -1998,7 +2035,7 @@
       <c r="AA4"/>
       <c r="AB4"/>
     </row>
-    <row r="5" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>11</v>
       </c>
@@ -2015,7 +2052,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="6" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>13</v>
       </c>
@@ -2032,7 +2069,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="7" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>9</v>
       </c>
@@ -2045,7 +2082,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>12</v>
       </c>
@@ -2058,50 +2095,292 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="9" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="12"/>
       <c r="F9" s="7"/>
       <c r="G9" s="7"/>
       <c r="H9" s="7"/>
     </row>
-    <row r="10" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="12"/>
       <c r="B10" s="12"/>
       <c r="F10" s="7"/>
       <c r="G10" s="7"/>
       <c r="H10" s="7"/>
     </row>
-    <row r="11" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="12"/>
       <c r="B11" s="12"/>
       <c r="F11" s="7"/>
       <c r="G11" s="7"/>
       <c r="H11" s="7"/>
     </row>
-    <row r="12" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="12"/>
       <c r="F12" s="7"/>
       <c r="G12" s="7"/>
       <c r="H12" s="7"/>
     </row>
-    <row r="13" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12"/>
       <c r="F13" s="7"/>
       <c r="G13" s="7"/>
       <c r="H13" s="7"/>
     </row>
-    <row r="14" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="12"/>
       <c r="B14" s="12"/>
       <c r="H14" s="13"/>
     </row>
-    <row r="15" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="12"/>
       <c r="B15" s="12"/>
       <c r="H15" s="13"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A12:B13">
+    <cfRule type="cellIs" dxfId="7" priority="4" operator="equal">
+      <formula>"class"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A14">
+    <cfRule type="cellIs" dxfId="6" priority="2" operator="equal">
+      <formula>"class"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A10:B11 A4:B4">
+    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
+      <formula>"class"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A15">
+    <cfRule type="cellIs" dxfId="4" priority="1" operator="equal">
+      <formula>"class"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AF51C9E-13CA-4D7E-BC08-059C6398D2DA}">
+  <sheetPr>
+    <tabColor rgb="FFFF9999"/>
+  </sheetPr>
+  <dimension ref="A1:AB15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <selection activeCell="D33" sqref="D33"/>
+      <selection pane="topRight" activeCell="D33" sqref="D33"/>
+      <selection pane="bottomLeft" activeCell="D33" sqref="D33"/>
+      <selection pane="bottomRight" activeCell="H7" sqref="H7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.42578125" style="14" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" customWidth="1"/>
+    <col min="6" max="8" width="10" customWidth="1"/>
+    <col min="9" max="15" width="6.7109375" customWidth="1"/>
+    <col min="16" max="16" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="2" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="6" bestFit="1" customWidth="1"/>
+    <col min="20" max="26" width="7" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="6" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="4" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A1" s="1"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="I4"/>
+      <c r="J4"/>
+      <c r="K4"/>
+      <c r="L4"/>
+      <c r="M4"/>
+      <c r="N4"/>
+      <c r="O4"/>
+      <c r="P4"/>
+      <c r="R4"/>
+      <c r="S4"/>
+      <c r="T4"/>
+      <c r="U4"/>
+      <c r="V4"/>
+      <c r="W4"/>
+      <c r="X4"/>
+      <c r="Y4"/>
+      <c r="Z4"/>
+      <c r="AA4"/>
+      <c r="AB4"/>
+    </row>
+    <row r="5" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" s="7">
+        <v>0.05</v>
+      </c>
+      <c r="G5" s="7">
+        <v>0.6</v>
+      </c>
+      <c r="H5" s="7">
+        <v>0.19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" s="7">
+        <f>0.3-0.15</f>
+        <v>0.15</v>
+      </c>
+      <c r="G6" s="7">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="H6" s="7">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="12"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+    </row>
+    <row r="10" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="12"/>
+      <c r="B10" s="12"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+    </row>
+    <row r="11" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="12"/>
+      <c r="B11" s="12"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
+    </row>
+    <row r="12" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="12"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="7"/>
+    </row>
+    <row r="13" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="12"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="7"/>
+    </row>
+    <row r="14" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="12"/>
+      <c r="B14" s="12"/>
+      <c r="H14" s="13"/>
+    </row>
+    <row r="15" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="12"/>
+      <c r="B15" s="12"/>
+      <c r="H15" s="13"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="A12:B13">
     <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
       <formula>"class"</formula>
     </cfRule>

</xml_diff>